<commit_message>
feat: update VariantAnnotation resource
</commit_message>
<xml_diff>
--- a/output/observations-summary.xlsx
+++ b/output/observations-summary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="101">
   <si>
     <t>Profile</t>
   </si>
@@ -291,6 +291,15 @@
   </si>
   <si>
     <t>Variant Annotation</t>
+  </si>
+  <si>
+    <t>LOINC#LP91038-7</t>
+  </si>
+  <si>
+    <t>LOINC#LP70194-3</t>
+  </si>
+  <si>
+    <t>LOINC#93044-6</t>
   </si>
   <si>
     <t>Unified Medical Language System#C0035687</t>
@@ -439,7 +448,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K123"/>
+  <dimension ref="A1:K126"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -4668,7 +4677,7 @@
         <v>13</v>
       </c>
       <c r="H121" t="s" s="2">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="I121" t="s" s="2">
         <v>17</v>
@@ -4694,7 +4703,7 @@
         <v>13</v>
       </c>
       <c r="E122" t="s" s="2">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="F122" t="s" s="2">
         <v>13</v>
@@ -4703,7 +4712,7 @@
         <v>13</v>
       </c>
       <c r="H122" t="s" s="2">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I122" t="s" s="2">
         <v>17</v>
@@ -4717,36 +4726,141 @@
     </row>
     <row r="123">
       <c r="A123" t="s" s="2">
-        <v>94</v>
+        <v>13</v>
       </c>
       <c r="B123" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="C123" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="D123" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="E123" t="s" s="2">
         <v>95</v>
       </c>
-      <c r="C123" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="D123" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="E123" t="s" s="2">
+      <c r="F123" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="G123" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="H123" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I123" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="J123" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="K123" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="B124" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="C124" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="D124" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="E124" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="F124" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="G124" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="H124" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="I124" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="J124" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="K124" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="B125" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="C125" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="D125" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="E125" t="s" s="2">
         <v>96</v>
       </c>
-      <c r="F123" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="G123" t="s" s="2">
+      <c r="F125" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="G125" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="H125" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="I125" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="J125" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="K125" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="H123" t="s" s="2">
-        <v>23</v>
-      </c>
-      <c r="I123" t="s" s="2">
-        <v>17</v>
-      </c>
-      <c r="J123" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="K123" t="s" s="2">
+      <c r="B126" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="C126" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="D126" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="E126" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="F126" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="G126" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="H126" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="I126" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="J126" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="K126" t="s" s="2">
         <v>13</v>
       </c>
     </row>

</xml_diff>